<commit_message>
work on service token studio
</commit_message>
<xml_diff>
--- a/notes/pdVFS database structure.xlsx
+++ b/notes/pdVFS database structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george\postdoc\postdoc\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george\github\postdoc\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CE22C5-42C6-4168-900E-911611D11D6D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922870D3-1E54-4FE7-9057-6C2A5525A7D1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="20115" windowHeight="7320" activeTab="2" xr2:uid="{161AC008-48D0-4979-A63E-E318768C4B55}"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="20115" windowHeight="7320" activeTab="2" xr2:uid="{161AC008-48D0-4979-A63E-E318768C4B55}"/>
   </bookViews>
   <sheets>
     <sheet name="vfs db" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="72">
   <si>
     <t>pdvfs</t>
   </si>
@@ -206,9 +206,6 @@
     <t>services</t>
   </si>
   <si>
-    <t>tokencreated</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -230,13 +227,22 @@
     <t>INTEGER PRIMARY KEY AUTOINCREMENT</t>
   </si>
   <si>
-    <t>ssl_force</t>
-  </si>
-  <si>
     <t>ssl_certificate</t>
   </si>
   <si>
     <t>ssl_key</t>
+  </si>
+  <si>
+    <t>tokenissued</t>
+  </si>
+  <si>
+    <t>base64 encoded, if empty, prompts for password (if the application supports it)</t>
+  </si>
+  <si>
+    <t>if empty, prompts prompts for full login credentials (if the appliations supports it)</t>
+  </si>
+  <si>
+    <t>secure</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1114,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1122,7 @@
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="74.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1144,7 +1150,7 @@
         <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1181,7 +1187,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1189,7 +1195,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -1197,7 +1203,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -1205,7 +1211,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -1213,26 +1219,29 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -1240,7 +1249,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -1251,7 +1260,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1262,7 +1271,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>

</xml_diff>